<commit_message>
fix linkedlist and stack time complexity in remove(element) operation
</commit_message>
<xml_diff>
--- a/RawData-Collections/LinkedList.xlsx
+++ b/RawData-Collections/LinkedList.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Desktop\EstimateEnergyConsumptionOfJavaPrograms\RawData-Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A66255C2-177E-4B0A-9E37-DEAB7A79403A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A008AB52-C6AC-4AC2-8F5B-ECD34F677E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkedList" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -924,11 +924,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,7 +1011,7 @@
         <v>3.2113265989999999</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1">
         <v>5.1377760000000001E-3</v>
@@ -1049,7 +1049,7 @@
         <v>3.5906448360000001</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J3" s="1">
         <v>9.0411229999999999E-3</v>
@@ -1087,7 +1087,7 @@
         <v>3.2122650149999998</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J4" s="1">
         <v>1.4296025E-2</v>
@@ -1125,7 +1125,7 @@
         <v>3.2303619380000002</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J5" s="1">
         <v>1.4511748E-2</v>
@@ -1163,7 +1163,7 @@
         <v>3.5906448360000001</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J6" s="1">
         <v>1.5044332000000001E-2</v>
@@ -1201,7 +1201,7 @@
         <v>2.8287353519999998</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J7" s="1">
         <v>3.5315811000000003E-2</v>
@@ -1239,7 +1239,7 @@
         <v>3.0719451900000001</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J8" s="1">
         <v>9.9782350000000002E-3</v>
@@ -1277,7 +1277,7 @@
         <v>3.5906448360000001</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J9" s="1">
         <v>1.4457892E-2</v>
@@ -1315,7 +1315,7 @@
         <v>4.0715026859999996</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J10" s="1">
         <v>4.7616109999999998E-3</v>
@@ -1353,7 +1353,7 @@
         <v>3.211585999</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J11" s="1">
         <v>7.3909090000000002E-3</v>
@@ -1391,7 +1391,7 @@
         <v>3.5886764530000002</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J12" s="1">
         <v>3.3532599999999998E-3</v>
@@ -1429,7 +1429,7 @@
         <v>3.2134017940000001</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J13" s="1">
         <v>6.7933760000000003E-3</v>
@@ -1467,7 +1467,7 @@
         <v>3.822296143</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J14" s="1">
         <v>8.548188E-3</v>
@@ -1505,7 +1505,7 @@
         <v>3.2283782959999998</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J15" s="1">
         <v>2.3412560999999998E-2</v>
@@ -1543,7 +1543,7 @@
         <v>2.5906448360000001</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J16" s="1">
         <v>1.5711447E-2</v>
@@ -1581,7 +1581,7 @@
         <v>3.5906600950000001</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J17" s="1">
         <v>5.556999E-3</v>
@@ -1619,7 +1619,7 @@
         <v>3.209716797</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J18" s="1">
         <v>1.7569861999999999E-2</v>
@@ -1657,7 +1657,7 @@
         <v>2.970832825</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J19" s="1">
         <v>4.7784488E-2</v>
@@ -1695,7 +1695,7 @@
         <v>5.5061111450000002</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J20" s="1">
         <v>1.0235459000000001E-2</v>
@@ -1733,7 +1733,7 @@
         <v>2.3462676999999998</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J21" s="1">
         <v>8.6354399999999994E-3</v>
@@ -1771,7 +1771,7 @@
         <v>3.350212097</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J22" s="1">
         <v>1.3043664999999999E-2</v>
@@ -1809,7 +1809,7 @@
         <v>3.0737609859999999</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J23" s="1">
         <v>5.0231959999999997E-3</v>
@@ -1847,7 +1847,7 @@
         <v>3.5906600950000001</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J24" s="1">
         <v>5.3575890000000003E-3</v>
@@ -1885,7 +1885,7 @@
         <v>3.2096405030000001</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J25" s="1">
         <v>8.8805389999999998E-3</v>
@@ -1923,7 +1923,7 @@
         <v>6.3501663209999997</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J26" s="1">
         <v>7.8713710000000003E-3</v>
@@ -1961,7 +1961,7 @@
         <v>3.2118682860000001</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J27" s="1">
         <v>1.2715799999999999E-2</v>
@@ -1999,7 +1999,7 @@
         <v>3.5906600950000001</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J28" s="1">
         <v>1.5167082E-2</v>
@@ -2037,7 +2037,7 @@
         <v>3.5886917110000001</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J29" s="1">
         <v>1.6167081999999999E-2</v>
@@ -2075,7 +2075,7 @@
         <v>3.211914063</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J30" s="1">
         <v>4.3769424000000001E-2</v>
@@ -2113,7 +2113,7 @@
         <v>3.2214813229999999</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J31" s="1">
         <v>8.3023999999999997E-3</v>
@@ -2151,7 +2151,7 @@
         <v>3.5945510860000001</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J32" s="1">
         <v>4.1717079999999997E-3</v>
@@ -2189,7 +2189,7 @@
         <v>2.9693069460000001</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J33" s="1">
         <v>3.5595429999999997E-2</v>
@@ -2227,7 +2227,7 @@
         <v>3.081542969</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J34" s="1">
         <v>8.6581620000000005E-3</v>
@@ -2265,7 +2265,7 @@
         <v>4.0645217899999997</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J35" s="1">
         <v>1.8548265000000001E-2</v>
@@ -2303,7 +2303,7 @@
         <v>3.2122955320000002</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J36" s="1">
         <v>9.9483509999999994E-3</v>
@@ -2341,7 +2341,7 @@
         <v>3.3462829589999998</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J37" s="1">
         <v>2.1955733000000002E-2</v>
@@ -2379,7 +2379,7 @@
         <v>4.0668334960000001</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J38" s="1">
         <v>6.6559890000000002E-3</v>
@@ -2417,7 +2417,7 @@
         <v>3.5906448360000001</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J39" s="1">
         <v>8.1681740000000003E-3</v>
@@ -2455,7 +2455,7 @@
         <v>3.2138442989999998</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J40" s="1">
         <v>7.6396270000000004E-3</v>
@@ -2493,7 +2493,7 @@
         <v>3.5906677249999999</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J41" s="1">
         <v>9.6277600000000008E-3</v>
@@ -2531,7 +2531,7 @@
         <v>2.9694366460000001</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J42" s="1">
         <v>2.1208274999999999E-2</v>
@@ -2569,7 +2569,7 @@
         <v>3.8293380739999998</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J43" s="1">
         <v>1.2001925E-2</v>
@@ -2607,7 +2607,7 @@
         <v>3.3491516109999999</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J44" s="1">
         <v>1.4638323999999999E-2</v>
@@ -2645,7 +2645,7 @@
         <v>3.072280884</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J45" s="1">
         <v>6.6553380000000002E-3</v>
@@ -2683,7 +2683,7 @@
         <v>3.3482513429999998</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J46" s="1">
         <v>2.4868832E-2</v>
@@ -2721,7 +2721,7 @@
         <v>3.8214111329999998</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J47" s="1">
         <v>1.6257402000000001E-2</v>
@@ -2759,7 +2759,7 @@
         <v>3.2117309569999999</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J48" s="1">
         <v>2.1243624999999999E-2</v>
@@ -2797,7 +2797,7 @@
         <v>2.969337463</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J49" s="1">
         <v>1.102498E-2</v>
@@ -2835,7 +2835,7 @@
         <v>3.5886764530000002</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J50" s="1">
         <v>5.3010440000000004E-3</v>
@@ -2873,7 +2873,7 @@
         <v>3.224235535</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J51" s="1">
         <v>1.0535048E-2</v>
@@ -2911,7 +2911,7 @@
         <v>3.5906448360000001</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J52" s="1">
         <v>2.5679779999999998E-3</v>
@@ -2949,7 +2949,7 @@
         <v>2.9879379269999999</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J53" s="1">
         <v>1.0820840999999999E-2</v>
@@ -2987,7 +2987,7 @@
         <v>3.2112350460000001</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J54" s="1">
         <v>8.1618709999999994E-3</v>
@@ -3025,7 +3025,7 @@
         <v>3.2118148799999999</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J55" s="1">
         <v>6.006852E-3</v>
@@ -3063,7 +3063,7 @@
         <v>3.2117309569999999</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J56" s="1">
         <v>3.1613990000000001E-3</v>
@@ -3101,7 +3101,7 @@
         <v>2.9689178470000002</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J57" s="1">
         <v>6.2106100000000001E-3</v>
@@ -3139,7 +3139,7 @@
         <v>3.2090377810000001</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J58" s="1">
         <v>1.8253100000000001E-2</v>
@@ -3177,7 +3177,7 @@
         <v>3.2132568359999998</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J59" s="1">
         <v>1.2944358E-2</v>
@@ -3215,7 +3215,7 @@
         <v>6.3521423339999998</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J60" s="1">
         <v>1.6303281999999999E-2</v>
@@ -3253,7 +3253,7 @@
         <v>3.0846557620000001</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J61" s="1">
         <v>1.7648484999999998E-2</v>
@@ -3291,7 +3291,7 @@
         <v>2.96925354</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J62" s="1">
         <v>5.6775599999999999E-3</v>
@@ -3329,7 +3329,7 @@
         <v>3.070213318</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J63" s="1">
         <v>2.2271503000000002E-2</v>
@@ -3367,7 +3367,7 @@
         <v>2.8267364499999998</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J64" s="1">
         <v>1.0542297000000001E-2</v>
@@ -3405,7 +3405,7 @@
         <v>2.842384338</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J65" s="1">
         <v>1.1900859999999999E-2</v>
@@ -3443,7 +3443,7 @@
         <v>2.8452835080000001</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J66" s="1">
         <v>7.7153889999999996E-3</v>
@@ -3481,7 +3481,7 @@
         <v>3.0712356569999999</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J67" s="1">
         <v>1.5607483E-2</v>
@@ -3519,7 +3519,7 @@
         <v>2.5906600950000001</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J68" s="1">
         <v>1.4316420999999999E-2</v>
@@ -3557,7 +3557,7 @@
         <v>5.8019332889999999</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J69" s="1">
         <v>9.8783829999999993E-3</v>
@@ -3595,7 +3595,7 @@
         <v>3.070411682</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J70" s="1">
         <v>6.8702210000000001E-3</v>
@@ -3633,7 +3633,7 @@
         <v>3.208984375</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J71" s="1">
         <v>1.0015542000000001E-2</v>
@@ -3671,7 +3671,7 @@
         <v>2.9691848749999998</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J72" s="1">
         <v>9.9396339999999993E-3</v>
@@ -3709,7 +3709,7 @@
         <v>3.8267517089999998</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J73" s="1">
         <v>8.2079860000000004E-3</v>
@@ -3747,7 +3747,7 @@
         <v>2.8318328859999999</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J74" s="1">
         <v>6.3560400000000003E-3</v>
@@ -3785,7 +3785,7 @@
         <v>3.0705947880000002</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J75" s="1">
         <v>1.5853874E-2</v>
@@ -3823,7 +3823,7 @@
         <v>5.9473953249999996</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J76" s="1">
         <v>1.5203339999999999E-2</v>
@@ -3861,7 +3861,7 @@
         <v>3.0742416380000002</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J77" s="1">
         <v>2.4000739E-2</v>
@@ -3899,7 +3899,7 @@
         <v>2.9879302980000002</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J78" s="1">
         <v>2.733311E-3</v>
@@ -3937,7 +3937,7 @@
         <v>3.3482360839999998</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J79" s="1">
         <v>2.7742498000000001E-2</v>
@@ -3975,7 +3975,7 @@
         <v>2.8257751459999998</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J80" s="1">
         <v>1.2991272E-2</v>
@@ -4013,7 +4013,7 @@
         <v>2.8472442629999999</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J81" s="1">
         <v>1.2615437E-2</v>
@@ -4051,7 +4051,7 @@
         <v>2.9714965819999999</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J82" s="1">
         <v>8.8060949999999999E-3</v>
@@ -4089,7 +4089,7 @@
         <v>2.9699630739999998</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J83" s="1">
         <v>1.49804E-2</v>
@@ -4127,7 +4127,7 @@
         <v>3.5886917110000001</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J84" s="1">
         <v>2.3861413000000001E-2</v>
@@ -4165,7 +4165,7 @@
         <v>2.9678115840000001</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J85" s="1">
         <v>1.0934723E-2</v>
@@ -4203,7 +4203,7 @@
         <v>3.5867080690000002</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J86" s="1">
         <v>6.1062119999999998E-3</v>
@@ -4241,7 +4241,7 @@
         <v>2.9697799680000001</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J87" s="1">
         <v>1.7908940000000002E-2</v>
@@ -4279,7 +4279,7 @@
         <v>3.2117462159999999</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J88" s="1">
         <v>5.3789770000000001E-3</v>
@@ -4317,7 +4317,7 @@
         <v>2.9693069460000001</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J89" s="1">
         <v>1.060533E-2</v>
@@ -4355,7 +4355,7 @@
         <v>6.5886764529999997</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J90" s="1">
         <v>4.2315098000000002E-2</v>
@@ -4393,7 +4393,7 @@
         <v>3.3501892089999998</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J91" s="1">
         <v>2.9913179000000002E-2</v>
@@ -4431,7 +4431,7 @@
         <v>3.3502197269999998</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J92" s="1">
         <v>2.5005550000000001E-2</v>
@@ -4469,7 +4469,7 @@
         <v>2.9684524539999999</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J93" s="1">
         <v>9.1306400000000006E-3</v>
@@ -4507,7 +4507,7 @@
         <v>3.2291870120000001</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J94" s="1">
         <v>1.3371144999999999E-2</v>
@@ -4545,7 +4545,7 @@
         <v>3.0720825199999999</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J95" s="1">
         <v>1.4982181000000001E-2</v>
@@ -4583,7 +4583,7 @@
         <v>3.5906448360000001</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J96" s="1">
         <v>5.0296585999999997E-2</v>
@@ -4621,7 +4621,7 @@
         <v>3.5886764530000002</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J97" s="1">
         <v>1.0681904000000001E-2</v>
@@ -4659,7 +4659,7 @@
         <v>2.9694366460000001</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J98" s="1">
         <v>7.1585499999999996E-3</v>
@@ -4697,7 +4697,7 @@
         <v>2.5590286249999998</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J99" s="1">
         <v>6.4691169999999999E-3</v>
@@ -4735,7 +4735,7 @@
         <v>3.0739669799999998</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J100" s="1">
         <v>8.4644130000000005E-3</v>
@@ -4773,7 +4773,7 @@
         <v>3.209701538</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J101" s="1">
         <v>5.624057E-3</v>

</xml_diff>